<commit_message>
Fix Mening test cases - Move Menactra to 10 years valid
Fixed Mening test cases - Moved Menactra to 10 years valid
All cases pass
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/Mening.xlsx
+++ b/src/main/webapp/schedules/Mening.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenyon\Documents\GitHub\LoneStarVaccineForecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F61D38-813D-4071-B546-2B6A1219869C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8E7B55-FBD6-4A30-B55E-07E87F3C92F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="396" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="396" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="216">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -191,9 +196,6 @@
     <t>Menactra</t>
   </si>
   <si>
-    <t>Menactra not licensed before 9 months.</t>
-  </si>
-  <si>
     <t>MPSV4 not licensed before 2 years.</t>
   </si>
   <si>
@@ -218,9 +220,6 @@
     <t>16 years -4 days</t>
   </si>
   <si>
-    <t>9 months -4 days</t>
-  </si>
-  <si>
     <t>2 months -4 days</t>
   </si>
   <si>
@@ -711,6 +710,9 @@
   </si>
   <si>
     <t>114, 147, 136</t>
+  </si>
+  <si>
+    <t>Menactra allowed earlier but not valid before 10 years of age</t>
   </si>
 </sst>
 </file>
@@ -880,9 +882,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -909,10 +911,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -927,7 +929,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1466,13 +1467,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1483,7 +1484,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1494,7 +1495,7 @@
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1505,7 +1506,7 @@
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1513,10 +1514,10 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1527,7 +1528,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1538,7 +1539,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1549,7 +1550,7 @@
         <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,7 +1561,7 @@
         <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1571,7 +1572,7 @@
         <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1582,7 +1583,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1590,10 +1591,10 @@
         <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1604,7 +1605,7 @@
         <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1615,7 +1616,7 @@
         <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,7 +1627,7 @@
         <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1637,7 +1638,7 @@
         <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1648,7 +1649,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1659,7 +1660,7 @@
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1670,7 +1671,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1681,7 +1682,7 @@
         <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1692,7 +1693,7 @@
         <v>146</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1703,7 +1704,7 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1714,7 +1715,7 @@
         <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1725,7 +1726,7 @@
         <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1736,7 +1737,7 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1744,10 +1745,10 @@
         <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1758,7 +1759,7 @@
         <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1769,7 +1770,7 @@
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1780,7 +1781,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1791,7 +1792,7 @@
         <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1802,7 +1803,7 @@
         <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1810,10 +1811,10 @@
         <v>158</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1824,7 +1825,7 @@
         <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1832,10 +1833,10 @@
         <v>160</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1843,10 +1844,10 @@
         <v>161</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1854,10 +1855,10 @@
         <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1868,7 +1869,7 @@
         <v>215</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1879,7 +1880,7 @@
         <v>216</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1887,10 +1888,10 @@
         <v>171</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1901,7 +1902,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1912,7 +1913,7 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1923,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1934,7 +1935,7 @@
         <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1945,7 +1946,7 @@
         <v>155</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1956,7 +1957,7 @@
         <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1967,7 +1968,7 @@
         <v>111</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1978,7 +1979,7 @@
         <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1989,7 +1990,7 @@
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2000,7 +2001,7 @@
         <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2011,7 +2012,7 @@
         <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2022,7 +2023,7 @@
         <v>147</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2033,7 +2034,7 @@
         <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2044,7 +2045,7 @@
         <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2055,7 +2056,7 @@
         <v>125</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2066,7 +2067,7 @@
         <v>126</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2077,7 +2078,7 @@
         <v>127</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2088,7 +2089,7 @@
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2099,7 +2100,7 @@
         <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2110,7 +2111,7 @@
         <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2121,7 +2122,7 @@
         <v>141</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2132,7 +2133,7 @@
         <v>166</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2143,7 +2144,7 @@
         <v>144</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2154,7 +2155,7 @@
         <v>149</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,7 +2166,7 @@
         <v>151</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2176,7 +2177,7 @@
         <v>150</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2187,7 +2188,7 @@
         <v>158</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2198,7 +2199,7 @@
         <v>119</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,7 +2210,7 @@
         <v>116</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2220,7 +2221,7 @@
         <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2231,7 +2232,7 @@
         <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2242,7 +2243,7 @@
         <v>18</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2253,7 +2254,7 @@
         <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,7 +2265,7 @@
         <v>90</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2275,7 +2276,7 @@
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,7 +2287,7 @@
         <v>122</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2297,7 +2298,7 @@
         <v>148</v>
       </c>
       <c r="C76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2308,7 +2309,7 @@
         <v>165</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,7 +2320,7 @@
         <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,7 +2331,7 @@
         <v>163</v>
       </c>
       <c r="C79" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2341,7 +2342,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2352,7 +2353,7 @@
         <v>118</v>
       </c>
       <c r="C81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2363,7 +2364,7 @@
         <v>137</v>
       </c>
       <c r="C82" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2374,7 +2375,7 @@
         <v>54</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2385,7 +2386,7 @@
         <v>55</v>
       </c>
       <c r="C84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2396,7 +2397,7 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2407,7 +2408,7 @@
         <v>24</v>
       </c>
       <c r="C86" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2418,7 +2419,7 @@
         <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2429,7 +2430,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2440,7 +2441,7 @@
         <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2451,7 +2452,7 @@
         <v>56</v>
       </c>
       <c r="C90" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2462,7 +2463,7 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2473,7 +2474,7 @@
         <v>102</v>
       </c>
       <c r="C92" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2484,7 +2485,7 @@
         <v>57</v>
       </c>
       <c r="C93" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2495,7 +2496,7 @@
         <v>52</v>
       </c>
       <c r="C94" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2506,7 +2507,7 @@
         <v>83</v>
       </c>
       <c r="C95" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2517,7 +2518,7 @@
         <v>84</v>
       </c>
       <c r="C96" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2528,7 +2529,7 @@
         <v>30</v>
       </c>
       <c r="C97" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2536,10 +2537,10 @@
         <v>1240</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C98" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2550,7 +2551,7 @@
         <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2561,7 +2562,7 @@
         <v>43</v>
       </c>
       <c r="C100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2572,7 +2573,7 @@
         <v>44</v>
       </c>
       <c r="C101" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2583,7 +2584,7 @@
         <v>59</v>
       </c>
       <c r="C102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2594,7 +2595,7 @@
         <v>60</v>
       </c>
       <c r="C103" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2605,7 +2606,7 @@
         <v>46</v>
       </c>
       <c r="C104" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2616,7 +2617,7 @@
         <v>47</v>
       </c>
       <c r="C105" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2627,7 +2628,7 @@
         <v>48</v>
       </c>
       <c r="C106" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2638,7 +2639,7 @@
         <v>49</v>
       </c>
       <c r="C107" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2649,7 +2650,7 @@
         <v>86</v>
       </c>
       <c r="C108" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2660,7 +2661,7 @@
         <v>87</v>
       </c>
       <c r="C109" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2671,7 +2672,7 @@
         <v>14</v>
       </c>
       <c r="C110" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2682,7 +2683,7 @@
         <v>39</v>
       </c>
       <c r="C111" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2693,7 +2694,7 @@
         <v>134</v>
       </c>
       <c r="C112" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2704,7 +2705,7 @@
         <v>64</v>
       </c>
       <c r="C113" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2715,7 +2716,7 @@
         <v>65</v>
       </c>
       <c r="C114" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2726,7 +2727,7 @@
         <v>67</v>
       </c>
       <c r="C115" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2737,7 +2738,7 @@
         <v>68</v>
       </c>
       <c r="C116" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -2748,7 +2749,7 @@
         <v>69</v>
       </c>
       <c r="C117" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2759,7 +2760,7 @@
         <v>11</v>
       </c>
       <c r="C118" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2770,7 +2771,7 @@
         <v>23</v>
       </c>
       <c r="C119" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2781,7 +2782,7 @@
         <v>70</v>
       </c>
       <c r="C120" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2792,7 +2793,7 @@
         <v>72</v>
       </c>
       <c r="C121" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -2803,7 +2804,7 @@
         <v>73</v>
       </c>
       <c r="C122" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -2814,7 +2815,7 @@
         <v>34</v>
       </c>
       <c r="C123" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -2825,7 +2826,7 @@
         <v>71</v>
       </c>
       <c r="C124" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -2836,7 +2837,7 @@
         <v>93</v>
       </c>
       <c r="C125" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -2847,7 +2848,7 @@
         <v>75</v>
       </c>
       <c r="C126" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -2858,7 +2859,7 @@
         <v>76</v>
       </c>
       <c r="C127" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -2869,7 +2870,7 @@
         <v>35</v>
       </c>
       <c r="C128" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -2880,7 +2881,7 @@
         <v>77</v>
       </c>
       <c r="C129" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -2891,7 +2892,7 @@
         <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -2902,7 +2903,7 @@
         <v>95</v>
       </c>
       <c r="C131" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -2913,7 +2914,7 @@
         <v>96</v>
       </c>
       <c r="C132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -2924,7 +2925,7 @@
         <v>97</v>
       </c>
       <c r="C133" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -2935,7 +2936,7 @@
         <v>98</v>
       </c>
       <c r="C134" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -2946,7 +2947,7 @@
         <v>78</v>
       </c>
       <c r="C135" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -2957,7 +2958,7 @@
         <v>25</v>
       </c>
       <c r="C136" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -2968,7 +2969,7 @@
         <v>41</v>
       </c>
       <c r="C137" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -2979,7 +2980,7 @@
         <v>53</v>
       </c>
       <c r="C138" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -2990,7 +2991,7 @@
         <v>101</v>
       </c>
       <c r="C139" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -3001,7 +3002,7 @@
         <v>91</v>
       </c>
       <c r="C140" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -3012,7 +3013,7 @@
         <v>79</v>
       </c>
       <c r="C141" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -3023,7 +3024,7 @@
         <v>81</v>
       </c>
       <c r="C142" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -3034,7 +3035,7 @@
         <v>80</v>
       </c>
       <c r="C143" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -3045,7 +3046,7 @@
         <v>92</v>
       </c>
       <c r="C144" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -3056,7 +3057,7 @@
         <v>36</v>
       </c>
       <c r="C145" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -3067,7 +3068,7 @@
         <v>37</v>
       </c>
       <c r="C146" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -3078,7 +3079,7 @@
         <v>121</v>
       </c>
       <c r="C147" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -3089,7 +3090,7 @@
         <v>131</v>
       </c>
       <c r="C148" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -3100,7 +3101,7 @@
         <v>133</v>
       </c>
       <c r="C149" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -3111,7 +3112,7 @@
         <v>999</v>
       </c>
       <c r="C150" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3124,7 +3125,7 @@
   <dimension ref="B1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3153,13 +3154,13 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -3172,8 +3173,8 @@
       <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="8"/>
       <c r="J3" s="6" t="s">
         <v>5</v>
@@ -3184,14 +3185,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D4" s="11"/>
       <c r="F4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
+        <v>112</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="11"/>
       <c r="J4" s="9">
         <v>32</v>
@@ -3206,10 +3207,10 @@
       </c>
       <c r="D5" s="11"/>
       <c r="F5" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="11"/>
       <c r="J5" s="9">
         <v>103</v>
@@ -3224,10 +3225,10 @@
       </c>
       <c r="D6" s="11"/>
       <c r="F6" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="22"/>
+        <v>113</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="11"/>
       <c r="J6" s="9">
         <v>114</v>
@@ -3242,10 +3243,10 @@
       </c>
       <c r="D7" s="11"/>
       <c r="F7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
+        <v>115</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="11"/>
       <c r="J7" s="9">
         <v>147</v>
@@ -3256,10 +3257,10 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="F8" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="11"/>
       <c r="J8" s="9">
         <v>136</v>
@@ -3351,12 +3352,12 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
@@ -3417,7 +3418,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -3443,11 +3444,11 @@
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
@@ -3471,10 +3472,10 @@
         <v>36</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>43</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
@@ -3485,10 +3486,10 @@
         <v>36</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -3499,10 +3500,10 @@
         <v>36</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
@@ -3513,10 +3514,10 @@
         <v>13</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
@@ -3527,10 +3528,10 @@
         <v>13</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
@@ -3541,7 +3542,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42" s="18"/>
     </row>
@@ -3554,7 +3555,7 @@
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
@@ -3609,12 +3610,12 @@
       <c r="D49" s="14"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="26"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="15"/>
@@ -3675,7 +3676,7 @@
         <v>26</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
@@ -3701,11 +3702,11 @@
       <c r="E58" s="9"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="26"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="25"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
@@ -3729,10 +3730,10 @@
         <v>33</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
@@ -3744,7 +3745,7 @@
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
@@ -3840,7 +3841,7 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="str">
+      <c r="A6" s="19" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B25&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C25&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D25&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E24&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
@@ -3852,103 +3853,103 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="str">
+      <c r="A8" s="19" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C28&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D28&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="8 weeks" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="str">
+      <c r="A9" s="19" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E29&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="str">
+      <c r="A10" s="19" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C30&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D30&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="str">
+      <c r="A11" s="19" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E31&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="str">
+      <c r="A12" s="19" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="str">
+      <c r="A13" s="19" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="str">
+      <c r="A14" s="19" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="str">
+      <c r="A15" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B37&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months -4 days" reason="Menactra not licensed before 9 months."/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="10 years" reason="Menactra allowed earlier but not valid before 10 years of age"/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="str">
+      <c r="A16" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B38&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years -4 days" reason="MPSV4 not licensed before 2 years."/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="str">
+      <c r="A17" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menveo" schedule="INVALID" age="2 months -4 days" reason="Menveo not licensed before 2 months."/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="str">
+      <c r="A18" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B40&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C40&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A1" age="10 years" reason="Received dose of MCV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="str">
+      <c r="A19" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A1" age="10 years" reason="Received dose of MPSV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="str">
+      <c r="A20" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B42&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="str">
+      <c r="A21" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B43&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="" reason="MPSV4 does not count for 16 year old dose"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="str">
+      <c r="A22" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B44&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D44&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E44&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="str">
+      <c r="A23" s="19" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="str">
+      <c r="A24" s="19" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B49&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C49&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D49&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E48&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
@@ -3960,150 +3961,150 @@
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="str">
+      <c r="A26" s="19" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="str">
+      <c r="A27" s="19" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="str">
+      <c r="A28" s="19" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="str">
+      <c r="A29" s="19" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="str">
+      <c r="A30" s="19" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="str">
+      <c r="A31" s="19" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="str">
+      <c r="A32" s="19" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="str">
+      <c r="A33" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B61&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C61&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D61&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="str">
+      <c r="A34" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="" reason="MPSV4 does not count for 16 year old dose"/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="str">
+      <c r="A35" s="19" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B63&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D63&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E63&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="str">
+      <c r="A36" s="19" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
-        <v>50</v>
+      <c r="A37" s="19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="19"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="19"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
+      <c r="A41" s="19"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="19"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
+      <c r="A46" s="19"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
+      <c r="A47" s="19"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
+      <c r="A55" s="19"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+      <c r="A56" s="19"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
+      <c r="A57" s="19"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
+      <c r="A58" s="19"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
+      <c r="A59" s="19"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
+      <c r="A60" s="19"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="20"/>
+      <c r="A61" s="19"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
+      <c r="A62" s="19"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>

</xml_diff>